<commit_message>
feat: support new services in mass uploading
</commit_message>
<xml_diff>
--- a/static/template.xlsx
+++ b/static/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladislavteli/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladislavteli/miranda/basic-oms/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E23D22-8215-1F43-9F13-26A231AC2EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F544377A-B572-7C43-A974-CC46AEC2E183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Тип населённого пункта</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>г.</t>
+  </si>
+  <si>
+    <t>Связанный заказ (СУЗ ID)</t>
+  </si>
+  <si>
+    <t>L2VPN</t>
   </si>
 </sst>
 </file>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -585,10 +591,11 @@
     <col min="7" max="7" width="36.83203125" style="10" customWidth="1"/>
     <col min="8" max="10" width="11.5" style="10" customWidth="1"/>
     <col min="11" max="12" width="14.6640625" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="10"/>
+    <col min="13" max="13" width="15.83203125" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="14" customFormat="1" ht="39" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -623,10 +630,13 @@
         <v>38</v>
       </c>
       <c r="L1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -649,7 +659,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>34</v>
@@ -658,11 +668,14 @@
         <v>1</v>
       </c>
       <c r="K2" s="13"/>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="13">
+        <v>12345</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -694,11 +707,12 @@
         <v>1</v>
       </c>
       <c r="K3" s="13"/>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="13"/>
+      <c r="M3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -728,11 +742,12 @@
         <v>1</v>
       </c>
       <c r="K4" s="13"/>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
@@ -764,11 +779,12 @@
         <v>1</v>
       </c>
       <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="13"/>
+      <c r="M5" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
@@ -802,13 +818,14 @@
       <c r="K6" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="13"/>
+      <c r="M6" s="13" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="8GzkZNEvgY1BxI2kW+zIjGfzuenjnXwESJwsqi2Cf4BiPjsaLF4Hen7KuR8Nl+OwS7lpY44TxClXopnGBdGifg==" saltValue="jWsRmKEt9KLAboQwPIAZbg==" spinCount="100000" sqref="D1:K1 L1:L6 H2:K6 A1:B6" name="Проектный офис"/>
+    <protectedRange algorithmName="SHA-512" hashValue="8GzkZNEvgY1BxI2kW+zIjGfzuenjnXwESJwsqi2Cf4BiPjsaLF4Hen7KuR8Nl+OwS7lpY44TxClXopnGBdGifg==" saltValue="jWsRmKEt9KLAboQwPIAZbg==" spinCount="100000" sqref="D1:K1 H2:K6 A1:B6 L1:M6" name="Проектный офис"/>
     <protectedRange algorithmName="SHA-512" hashValue="8GzkZNEvgY1BxI2kW+zIjGfzuenjnXwESJwsqi2Cf4BiPjsaLF4Hen7KuR8Nl+OwS7lpY44TxClXopnGBdGifg==" saltValue="jWsRmKEt9KLAboQwPIAZbg==" spinCount="100000" sqref="C1" name="Проектный офис_1"/>
     <protectedRange algorithmName="SHA-512" hashValue="8GzkZNEvgY1BxI2kW+zIjGfzuenjnXwESJwsqi2Cf4BiPjsaLF4Hen7KuR8Nl+OwS7lpY44TxClXopnGBdGifg==" saltValue="jWsRmKEt9KLAboQwPIAZbg==" spinCount="100000" sqref="C2:C6" name="Проектный офис_21"/>
     <protectedRange algorithmName="SHA-512" hashValue="8GzkZNEvgY1BxI2kW+zIjGfzuenjnXwESJwsqi2Cf4BiPjsaLF4Hen7KuR8Nl+OwS7lpY44TxClXopnGBdGifg==" saltValue="jWsRmKEt9KLAboQwPIAZbg==" spinCount="100000" sqref="D2:D6" name="Проектный офис_33"/>

</xml_diff>